<commit_message>
Fixed index error with Undo button
</commit_message>
<xml_diff>
--- a/Practice.xlsx
+++ b/Practice.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeok\PycharmProjects\TICounter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74756C45-CB8E-4F8C-A3A4-23F2BB9AD672}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E32CD-3825-476E-8DD0-7EF1A6FF9562}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="600" windowWidth="18216" windowHeight="10824" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="The Chase" sheetId="2" r:id="rId2"/>
     <sheet name="Tough Shoe" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="19">
   <si>
     <t>Board</t>
   </si>
@@ -78,6 +79,9 @@
   <si>
     <t>F8</t>
   </si>
+  <si>
+    <t>Total:</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +128,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -137,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -158,6 +174,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2650,7 +2674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
@@ -3434,4 +3458,463 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="13">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Total Profit display error
</commit_message>
<xml_diff>
--- a/Practice.xlsx
+++ b/Practice.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeok\PycharmProjects\TICounter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E32CD-3825-476E-8DD0-7EF1A6FF9562}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6245ED31-87CA-4619-B51E-7144A7DB7BC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="The Chase" sheetId="2" r:id="rId2"/>
     <sheet name="Tough Shoe" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="19">
   <si>
     <t>Board</t>
   </si>
@@ -2674,7 +2675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
@@ -3461,10 +3462,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
@@ -3917,4 +3918,490 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="13">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed count undo error
</commit_message>
<xml_diff>
--- a/Practice.xlsx
+++ b/Practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeok\PycharmProjects\TICounter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A37909-BD7C-479C-AA50-240FD1317DAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB61DDB-048E-426D-8B34-15655F87BB75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3948" yWindow="612" windowWidth="16584" windowHeight="11220" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3948" yWindow="612" windowWidth="16584" windowHeight="11220" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3026" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="29">
   <si>
     <t>Board</t>
   </si>
@@ -129,15 +129,6 @@
   </si>
   <si>
     <t>Banker</t>
-  </si>
-  <si>
-    <t>Checks</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>~</t>
   </si>
 </sst>
 </file>
@@ -10066,8 +10057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10085,9 +10076,6 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
@@ -10142,9 +10130,6 @@
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
       <c r="G7">
         <v>1</v>
       </c>
@@ -10159,9 +10144,6 @@
       <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
       <c r="G8">
         <v>-2</v>
       </c>
@@ -10175,9 +10157,6 @@
       </c>
       <c r="E9" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
       </c>
       <c r="G9">
         <v>-4</v>
@@ -10193,9 +10172,6 @@
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
       <c r="G10" s="10">
         <v>-1</v>
       </c>
@@ -10210,9 +10186,6 @@
       <c r="E11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
       <c r="G11">
         <v>1</v>
       </c>
@@ -10227,9 +10200,6 @@
       <c r="E12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
       <c r="G12" s="10">
         <v>4</v>
       </c>
@@ -10244,9 +10214,6 @@
       <c r="E13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
       <c r="G13">
         <v>1</v>
       </c>
@@ -10261,9 +10228,6 @@
       <c r="E14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
       <c r="G14" s="10">
         <v>4</v>
       </c>
@@ -10278,9 +10242,6 @@
       <c r="E15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
       <c r="G15">
         <v>1</v>
       </c>
@@ -10294,9 +10255,6 @@
       </c>
       <c r="E16" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
       </c>
       <c r="G16">
         <v>-2</v>
@@ -10312,9 +10270,6 @@
       <c r="E17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
       <c r="G17" s="10">
         <v>0</v>
       </c>
@@ -10328,9 +10283,6 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -10346,9 +10298,6 @@
       <c r="E19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
       <c r="G19" s="10">
         <v>4</v>
       </c>
@@ -10363,9 +10312,6 @@
       <c r="E20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
       <c r="G20">
         <v>-1</v>
       </c>
@@ -10380,9 +10326,6 @@
       <c r="E21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F21" t="s">
-        <v>31</v>
-      </c>
       <c r="G21" s="10">
         <v>1</v>
       </c>
@@ -10396,9 +10339,6 @@
       </c>
       <c r="E22" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>31</v>
       </c>
       <c r="G22">
         <v>-1</v>
@@ -10414,9 +10354,6 @@
       <c r="E23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F23" t="s">
-        <v>31</v>
-      </c>
       <c r="G23" s="10">
         <v>1</v>
       </c>
@@ -10431,9 +10368,6 @@
       <c r="E24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
       <c r="G24">
         <v>1</v>
       </c>
@@ -10447,9 +10381,6 @@
       </c>
       <c r="E25" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>30</v>
       </c>
       <c r="G25">
         <v>-2</v>
@@ -10465,9 +10396,6 @@
       <c r="E26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
       <c r="G26">
         <v>-4</v>
       </c>
@@ -10482,9 +10410,6 @@
       <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
       <c r="G27">
         <v>-7</v>
       </c>
@@ -10499,9 +10424,6 @@
       <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F28" t="s">
-        <v>30</v>
-      </c>
       <c r="G28" s="10">
         <v>-12</v>
       </c>
@@ -10515,9 +10437,6 @@
       </c>
       <c r="E29" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -10533,9 +10452,6 @@
       <c r="E30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F30" t="s">
-        <v>30</v>
-      </c>
       <c r="G30" s="10">
         <v>4</v>
       </c>
@@ -10549,9 +10465,6 @@
       </c>
       <c r="E31" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F31" t="s">
-        <v>30</v>
       </c>
       <c r="G31">
         <v>-1</v>
@@ -10567,9 +10480,6 @@
       <c r="E32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F32" t="s">
-        <v>31</v>
-      </c>
       <c r="G32" s="10">
         <v>1</v>
       </c>
@@ -10583,9 +10493,6 @@
       </c>
       <c r="E33" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F33" t="s">
-        <v>30</v>
       </c>
       <c r="G33">
         <v>-1</v>
@@ -10601,9 +10508,6 @@
       <c r="E34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F34" t="s">
-        <v>30</v>
-      </c>
       <c r="G34" s="10">
         <v>1</v>
       </c>
@@ -10618,9 +10522,6 @@
       <c r="E35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F35" t="s">
-        <v>31</v>
-      </c>
       <c r="G35">
         <v>1</v>
       </c>
@@ -10635,25 +10536,19 @@
       <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F36" t="s">
-        <v>31</v>
-      </c>
       <c r="G36" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>30</v>
       </c>
       <c r="G37">
         <v>-1</v>
@@ -10661,7 +10556,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>7</v>
@@ -10669,25 +10564,19 @@
       <c r="E38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F38" t="s">
-        <v>31</v>
-      </c>
       <c r="G38" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F39" t="s">
-        <v>31</v>
       </c>
       <c r="G39">
         <v>-1</v>
@@ -10695,7 +10584,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>7</v>
@@ -10703,25 +10592,19 @@
       <c r="E40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F40" t="s">
-        <v>31</v>
-      </c>
       <c r="G40" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>31</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -10729,7 +10612,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -10737,16 +10620,13 @@
       <c r="E42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F42" t="s">
-        <v>31</v>
-      </c>
       <c r="G42">
         <v>-2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -10754,16 +10634,13 @@
       <c r="E43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F43" t="s">
-        <v>31</v>
-      </c>
       <c r="G43">
         <v>-4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>8</v>
@@ -10771,25 +10648,19 @@
       <c r="E44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F44" t="s">
-        <v>31</v>
-      </c>
       <c r="G44" s="10">
         <v>-1</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>31</v>
       </c>
       <c r="G45">
         <v>-1</v>
@@ -10797,7 +10668,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>7</v>
@@ -10805,25 +10676,19 @@
       <c r="E46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F46" t="s">
-        <v>31</v>
-      </c>
       <c r="G46" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F47" t="s">
-        <v>30</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -10839,9 +10704,6 @@
       <c r="E48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F48" t="s">
-        <v>31</v>
-      </c>
       <c r="G48" s="10">
         <v>4</v>
       </c>
@@ -10856,16 +10718,13 @@
       <c r="E49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F49" t="s">
-        <v>31</v>
-      </c>
       <c r="G49">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -10873,9 +10732,6 @@
       <c r="E50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F50" t="s">
-        <v>30</v>
-      </c>
       <c r="G50">
         <v>-2</v>
       </c>
@@ -10889,9 +10745,6 @@
       </c>
       <c r="E51" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F51" t="s">
-        <v>31</v>
       </c>
       <c r="G51" s="10">
         <v>0</v>
@@ -10907,17 +10760,12 @@
       <c r="E52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F52" t="s">
-        <v>31</v>
-      </c>
       <c r="G52" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F53" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="F53" s="11"/>
       <c r="G53" s="12">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Undo button fixed (forreal)
</commit_message>
<xml_diff>
--- a/Practice.xlsx
+++ b/Practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeok\PycharmProjects\TICounter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB61DDB-048E-426D-8B34-15655F87BB75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D40B49-755B-4C8D-8B1C-30439A3A6F4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3948" yWindow="612" windowWidth="16584" windowHeight="11220" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="14" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,14 @@
     <sheet name="Sheet18" sheetId="21" r:id="rId21"/>
     <sheet name="Sheet19" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet20" sheetId="23" r:id="rId23"/>
+    <sheet name="#18 Revise" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="30">
   <si>
     <t>Board</t>
   </si>
@@ -129,6 +130,9 @@
   </si>
   <si>
     <t>Banker</t>
+  </si>
+  <si>
+    <t>Checks</t>
   </si>
 </sst>
 </file>
@@ -8615,7 +8619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -9077,7 +9083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
@@ -10057,8 +10063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10768,6 +10774,549 @@
       <c r="F53" s="11"/>
       <c r="G53" s="12">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>-1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="12">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>